<commit_message>
Fixed Program Not Running
</commit_message>
<xml_diff>
--- a/Practice Trial.xlsx
+++ b/Practice Trial.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24430"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24527"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/38ab04e5e41146aa/Desktop/research/Eating Observation Exp 2.0/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ranwei\Desktop\Eating Observation Exp 2.0\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="13" documentId="13_ncr:1_{66EF577A-8090-4E26-9E05-79CCAC7024FE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{4AC709E3-C859-4E2A-9360-957D16931C40}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8BA7A7E4-9E48-48BB-99B8-6602D2BC460B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1560" yWindow="1560" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -72,9 +72,6 @@
     <t>window</t>
   </si>
   <si>
-    <t>blue</t>
-  </si>
-  <si>
     <t>red</t>
   </si>
   <si>
@@ -87,7 +84,10 @@
     <t>green</t>
   </si>
   <si>
-    <t>black</t>
+    <t>deepskyblue</t>
+  </si>
+  <si>
+    <t>gold</t>
   </si>
 </sst>
 </file>
@@ -408,17 +408,17 @@
   <dimension ref="A1:B16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H9" sqref="H9"/>
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
@@ -426,7 +426,7 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>15</v>
+        <v>19</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
@@ -434,7 +434,7 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
@@ -442,7 +442,7 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
@@ -450,7 +450,7 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
@@ -466,7 +466,7 @@
         <v>0</v>
       </c>
       <c r="B7" t="s">
-        <v>15</v>
+        <v>19</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
@@ -474,7 +474,7 @@
         <v>6</v>
       </c>
       <c r="B8" t="s">
-        <v>15</v>
+        <v>19</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
@@ -482,7 +482,7 @@
         <v>7</v>
       </c>
       <c r="B9" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
@@ -498,7 +498,7 @@
         <v>9</v>
       </c>
       <c r="B11" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
@@ -514,7 +514,7 @@
         <v>11</v>
       </c>
       <c r="B13" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
@@ -530,7 +530,7 @@
         <v>13</v>
       </c>
       <c r="B15" t="s">
-        <v>15</v>
+        <v>19</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
@@ -538,7 +538,7 @@
         <v>14</v>
       </c>
       <c r="B16" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
   </sheetData>

</xml_diff>